<commit_message>
Agregaciones Plantilla y carga de archivo
</commit_message>
<xml_diff>
--- a/schedule-management-backend/src/main/resources/files/templates/Plantilla_Ambientes.xlsx
+++ b/schedule-management-backend/src/main/resources/files/templates/Plantilla_Ambientes.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Documents\202301\proyecto1\Corte1\cloncorte2\schedule-management-unicauca\schedule-management-backend\src\main\resources\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Documents\202301\proyecto1\Corte1\cloncorteoriginal\schedule-management-unicauca\schedule-management-backend\src\main\resources\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD19FA9-3120-4EB6-8D36-94018322AA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772C50B3-F77F-4B36-8E60-B8D8A46B98CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FDB89DEF-8F0C-4572-A7F8-3E2FCA9F9031}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -220,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -242,12 +243,26 @@
   <si>
     <t>CANTIDAD</t>
   </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Salon</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t>Edificio</t>
+  </si>
+  <si>
+    <t>Auditorio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -325,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -338,6 +353,14 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -654,21 +677,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330A7A7F-241B-42C4-A065-E8DCD7CF59C6}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.140625"/>
-    <col min="2" max="2" customWidth="true" width="15.0"/>
-    <col min="3" max="3" customWidth="true" style="4" width="15.5703125"/>
-    <col min="4" max="4" customWidth="true" width="13.28515625"/>
-    <col min="5" max="5" customWidth="true" width="10.0"/>
-    <col min="6" max="6" customWidth="true" width="22.85546875"/>
-    <col min="7" max="7" customWidth="true" style="5" width="16.7109375"/>
+    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -694,10 +717,513 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="9"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="9"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="9"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="9"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="9"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="9"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="9"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="9"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="9"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="9"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="9"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="9"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="9"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="9"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="9"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="9"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3AD9774D-9FF1-4400-B2B8-3828324770F9}">
+          <x14:formula1>
+            <xm:f>Hoja2!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D51</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D148A48A-1F01-4924-91F1-2283DB9A9431}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
integracion de subida de archivo para ambiente
</commit_message>
<xml_diff>
--- a/schedule-management-backend/src/main/resources/files/templates/Plantilla_Ambientes.xlsx
+++ b/schedule-management-backend/src/main/resources/files/templates/Plantilla_Ambientes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Documents\202301\proyecto1\Corte1\cloncorteoriginal\schedule-management-unicauca\schedule-management-backend\src\main\resources\files\templates\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -263,6 +263,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -685,13 +686,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.140625"/>
+    <col min="2" max="2" customWidth="true" width="15.0"/>
+    <col min="3" max="3" customWidth="true" style="4" width="15.5703125"/>
+    <col min="4" max="4" customWidth="true" width="13.28515625"/>
+    <col min="5" max="5" customWidth="true" width="10.0"/>
+    <col min="6" max="6" customWidth="true" width="22.85546875"/>
+    <col min="7" max="7" customWidth="true" style="5" width="16.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1173,7 +1174,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3AD9774D-9FF1-4400-B2B8-3828324770F9}">
           <x14:formula1>

</xml_diff>

<commit_message>
Cambios en plantilla ambientes
</commit_message>
<xml_diff>
--- a/schedule-management-backend/src/main/resources/files/templates/Plantilla_Ambientes.xlsx
+++ b/schedule-management-backend/src/main/resources/files/templates/Plantilla_Ambientes.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Documents\202301\proyecto1\Corte1\cloncorteoriginal\schedule-management-unicauca\schedule-management-backend\src\main\resources\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Documents\202301\proyecto1\Corte2\schedule-management-unicauca\schedule-management-backend\src\main\resources\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772C50B3-F77F-4B36-8E60-B8D8A46B98CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AD0283-CF58-44EA-B023-7DFD51379A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FDB89DEF-8F0C-4572-A7F8-3E2FCA9F9031}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="AMBIENTES" sheetId="1" r:id="rId1"/>
+    <sheet name="ESPECIFICACIONES" sheetId="4" r:id="rId2"/>
+    <sheet name="CONSULTAS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -216,12 +217,223 @@
         </r>
       </text>
     </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{46B32A24-5F8E-4524-9DF1-7EC416C8BA9F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Recursos adicionales del ambiente:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+-Digite los recursos que tenga el ambiente separados por una coma.
+-Los recursos digitados deben estar previamente creados en la opcion agregar recursos de la aplicacion.
+-Si es un edificio se digita: 'no aplica'</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Windows 10</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{918E54E0-9067-4A6D-AECA-428C19A7E59C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nombre del ambiente: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">-Se aceptan numeros de salones, caracteres o nombres generales.  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{5EB1B9FF-6F89-4554-9742-30B6450BF688}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Ubicacion del ambiente: 
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Para Edificios digitar: no aplica.
+- Para los demas digitar: el edifiicio donde se encuentra el ambiente.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{2B80E40A-1041-447F-81C5-4BED4F9C83C9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Capacidad del Ambiente:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">-Si es edificio 'no aplica', de lo contrario colocar la capacidad del ambiente.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{974C11A5-2847-49D7-8808-E26BDA16D557}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tipos de ambiente digite segun corresponda:
+-</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>laboratorio,salon,edificio,auditorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{7FD5087B-88A2-497F-86C0-0821789643C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Digite la facultad del ambiente: FIET,FIC</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6E119F3E-B5B0-495D-8D16-29163A4550C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Recursos adicionales del ambiente:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+-Digite los recursos que tenga el ambiente separados por una coma.
+-Los recursos digitados deben estar previamente creados en la opcion agregar recursos de la aplicacion.
+-Si es un edificio se digita: 'no aplica'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{A283E472-1826-401B-9045-E04A094C34A5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Cantidad de recursos adicionales:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>-Se digitan los recursos adicionales en numeros enteros, separados por una coma, ejemplo: 1,1.
+-si es edificio: 'no aplica'.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -244,9 +456,6 @@
     <t>CANTIDAD</t>
   </si>
   <si>
-    <t>Tipo</t>
-  </si>
-  <si>
     <t>Salon</t>
   </si>
   <si>
@@ -257,14 +466,52 @@
   </si>
   <si>
     <t>Auditorio</t>
+  </si>
+  <si>
+    <t>FIET</t>
+  </si>
+  <si>
+    <t>FACULTAD DE INGENIERIA ELECTRONICA Y DE COMUNICACIONES</t>
+  </si>
+  <si>
+    <t>FIC</t>
+  </si>
+  <si>
+    <t>FACULTAD DE INGENIERIA CIVIL</t>
+  </si>
+  <si>
+    <t>CODIGO</t>
+  </si>
+  <si>
+    <t>RECURSOS ADICIONALES DISPONIBLES</t>
+  </si>
+  <si>
+    <t>Video Beam</t>
+  </si>
+  <si>
+    <t>Televisor</t>
+  </si>
+  <si>
+    <t>Tipo De Ambientes</t>
+  </si>
+  <si>
+    <t>Campo</t>
+  </si>
+  <si>
+    <t>Especificacion</t>
+  </si>
+  <si>
+    <t>Ejemplo</t>
+  </si>
+  <si>
+    <t>Se aceptan numeros de salones o nombres</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,8 +546,23 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +572,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -363,6 +631,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,24 +970,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330A7A7F-241B-42C4-A065-E8DCD7CF59C6}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.140625"/>
-    <col min="2" max="2" customWidth="true" width="15.0"/>
-    <col min="3" max="3" customWidth="true" style="4" width="15.5703125"/>
-    <col min="4" max="4" customWidth="true" width="13.28515625"/>
-    <col min="5" max="5" customWidth="true" width="10.0"/>
-    <col min="6" max="6" customWidth="true" width="22.85546875"/>
-    <col min="7" max="7" customWidth="true" style="5" width="16.7109375"/>
+    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -717,8 +1010,11 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J1" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
@@ -726,8 +1022,11 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J2" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -735,8 +1034,11 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J3" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -744,8 +1046,9 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -753,8 +1056,9 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -762,8 +1066,9 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -771,8 +1076,9 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -780,8 +1086,9 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
@@ -789,8 +1096,9 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -798,8 +1106,9 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -807,8 +1116,9 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -816,8 +1126,9 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -825,8 +1136,9 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -834,8 +1146,9 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -843,8 +1156,9 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -852,8 +1166,9 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -861,8 +1176,9 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -870,8 +1186,9 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -879,8 +1196,9 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -888,8 +1206,9 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
@@ -897,8 +1216,9 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -906,8 +1226,9 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -915,8 +1236,9 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -924,8 +1246,9 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -933,8 +1256,9 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
@@ -942,8 +1266,9 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -951,8 +1276,9 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -960,8 +1286,9 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
@@ -969,8 +1296,9 @@
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
@@ -978,8 +1306,9 @@
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="9"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -987,8 +1316,9 @@
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="9"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -996,8 +1326,9 @@
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="9"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
@@ -1005,8 +1336,9 @@
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="9"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
@@ -1014,8 +1346,9 @@
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
@@ -1023,8 +1356,9 @@
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="9"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J35" s="7"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
@@ -1032,8 +1366,9 @@
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="9"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" s="7"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
@@ -1041,8 +1376,9 @@
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="9"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
@@ -1050,8 +1386,9 @@
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="9"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" s="7"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
@@ -1059,8 +1396,9 @@
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="9"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J39" s="7"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
@@ -1068,8 +1406,9 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="9"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J40" s="7"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
@@ -1077,8 +1416,9 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="9"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J41" s="7"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
@@ -1086,8 +1426,9 @@
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="9"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J42" s="7"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
@@ -1095,8 +1436,9 @@
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="9"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J43" s="7"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
@@ -1104,8 +1446,9 @@
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="9"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J44" s="7"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
@@ -1113,8 +1456,9 @@
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="9"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
@@ -1122,8 +1466,9 @@
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="9"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
@@ -1131,8 +1476,9 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="9"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J47" s="7"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
@@ -1140,8 +1486,9 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="9"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="8"/>
@@ -1149,8 +1496,9 @@
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="9"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J49" s="7"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
@@ -1158,8 +1506,9 @@
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="9"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J50" s="7"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
@@ -1167,6 +1516,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="9"/>
+      <c r="J51" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1174,11 +1524,17 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6AF341C7-0E8B-4088-BCA7-B71A4E918A36}">
+          <x14:formula1>
+            <xm:f>CONSULTAS!$A$2:$A$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E51</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3AD9774D-9FF1-4400-B2B8-3828324770F9}">
           <x14:formula1>
-            <xm:f>Hoja2!$A$2:$A$5</xm:f>
+            <xm:f>CONSULTAS!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D51</xm:sqref>
         </x14:dataValidation>
@@ -1189,42 +1545,385 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D148A48A-1F01-4924-91F1-2283DB9A9431}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51C9D736-7310-4A2E-A36F-E6626D36506D}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>11</v>
-      </c>
+    <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="4"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A010E52C-A240-4890-9DB7-404AE0E875E9}">
+          <x14:formula1>
+            <xm:f>CONSULTAS!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9FA72875-C813-4610-8532-95DCADBDA22F}">
+          <x14:formula1>
+            <xm:f>CONSULTAS!$A$2:$A$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B871DA-02F7-4B0C-AA3F-5422D277DFCC}">
+  <dimension ref="A1:E60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="59.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios en plantila ambientes y arreglos generales
</commit_message>
<xml_diff>
--- a/schedule-management-backend/src/main/resources/files/templates/Plantilla_Ambientes.xlsx
+++ b/schedule-management-backend/src/main/resources/files/templates/Plantilla_Ambientes.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Documents\202301\proyecto1\Corte2\schedule-management-unicauca\schedule-management-backend\src\main\resources\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AD0283-CF58-44EA-B023-7DFD51379A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C489B5-BA1B-4550-AB9D-8386FDC3F502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FDB89DEF-8F0C-4572-A7F8-3E2FCA9F9031}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">-Se aceptan numeros de salones, caracteres o nombres generales.  </t>
+          <t>-Se aceptan numeros de salones, caracteres o nombres generales.  
+Consulte ESPECIFICACIONES</t>
         </r>
       </text>
     </comment>
@@ -88,7 +89,8 @@
             <family val="2"/>
           </rPr>
           <t>Para Edificios digitar: no aplica.
-- Para los demas digitar: el edifiicio donde se encuentra el ambiente.</t>
+- Para los demas digitar: el edifiicio donde se encuentra el ambiente.
+Consulte ESPECIFICACIONES</t>
         </r>
       </text>
     </comment>
@@ -112,8 +114,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">-Si es edificio 'no aplica', de lo contrario colocar la capacidad del ambiente.
-</t>
+          <t>-Si es edificio 'no aplica', de lo contrario colocar la capacidad del ambiente.
+Consulte ESPECIFICACIONES</t>
         </r>
       </text>
     </comment>
@@ -137,7 +139,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>laboratorio,salon,edificio,auditorio</t>
+          <t>laboratorio,salon,edificio,auditorio
+Consulte ESPECIFICACIONES</t>
         </r>
       </text>
     </comment>
@@ -151,7 +154,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Digite la facultad del ambiente: FIET,FIC</t>
+          <t xml:space="preserve">Seleccione la facultad del ambiente: </t>
         </r>
         <r>
           <rPr>
@@ -161,7 +164,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+Consulte ESPECIFICACIONES</t>
         </r>
       </text>
     </comment>
@@ -188,7 +191,8 @@
           <t xml:space="preserve">
 -Digite los recursos que tenga el ambiente separados por una coma.
 -Los recursos digitados deben estar previamente creados en la opcion agregar recursos de la aplicacion.
--Si es un edificio se digita: 'no aplica'</t>
+-Si es un edificio se digita: 'no aplica'
+Consulte ESPECIFICACIONES</t>
         </r>
       </text>
     </comment>
@@ -213,7 +217,8 @@
             <family val="2"/>
           </rPr>
           <t>-Se digitan los recursos adicionales en numeros enteros, separados por una coma, ejemplo: 1,1.
--si es edificio: 'no aplica'.</t>
+-si es edificio: 'no aplica'.
+Consulte ESPECIFICACIONES</t>
         </r>
       </text>
     </comment>
@@ -227,8 +232,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Recursos adicionales del ambiente:
-</t>
+          <t>Recursos adicionales del ambiente:</t>
         </r>
         <r>
           <rPr>
@@ -238,9 +242,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
--Digite los recursos que tenga el ambiente separados por una coma.
 -Los recursos digitados deben estar previamente creados en la opcion agregar recursos de la aplicacion.
--Si es un edificio se digita: 'no aplica'</t>
+-En la lista se muestran los recursos disponibles que se pueden colocar uno o varios separados por una coma.</t>
         </r>
       </text>
     </comment>
@@ -278,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{5EB1B9FF-6F89-4554-9742-30B6450BF688}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{5EB1B9FF-6F89-4554-9742-30B6450BF688}">
       <text>
         <r>
           <rPr>
@@ -303,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{2B80E40A-1041-447F-81C5-4BED4F9C83C9}">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{2B80E40A-1041-447F-81C5-4BED4F9C83C9}">
       <text>
         <r>
           <rPr>
@@ -328,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{974C11A5-2847-49D7-8808-E26BDA16D557}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{974C11A5-2847-49D7-8808-E26BDA16D557}">
       <text>
         <r>
           <rPr>
@@ -352,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{7FD5087B-88A2-497F-86C0-0821789643C7}">
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{7FD5087B-88A2-497F-86C0-0821789643C7}">
       <text>
         <r>
           <rPr>
@@ -362,7 +365,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Digite la facultad del ambiente: FIET,FIC</t>
+          <t xml:space="preserve">Digite la facultad del ambiente: </t>
         </r>
         <r>
           <rPr>
@@ -376,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6E119F3E-B5B0-495D-8D16-29163A4550C8}">
+    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{6E119F3E-B5B0-495D-8D16-29163A4550C8}">
       <text>
         <r>
           <rPr>
@@ -403,7 +406,181 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{A283E472-1826-401B-9045-E04A094C34A5}">
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{A283E472-1826-401B-9045-E04A094C34A5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Cantidad de recursos adicionales:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>-Se digitan los recursos adicionales en numeros enteros, separados por una coma, ejemplo: 1,1.
+-si es edificio: 'no aplica'.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{5B0E9865-AFAD-4F88-B51C-EE6E15520C24}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nombre del ambiente: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">-Se aceptan numeros de salones, caracteres o nombres generales.  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{B583997F-0504-4223-9F2E-385339023A7B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Ubicacion del ambiente: 
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Para Edificios digitar: no aplica.
+- Para los demas digitar: el edifiicio donde se encuentra el ambiente.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{99A00706-3C11-4D49-A67A-CFF699E83A94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Capacidad del Ambiente:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">-Si es edificio 'no aplica', de lo contrario colocar la capacidad del ambiente.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E28" authorId="0" shapeId="0" xr:uid="{68BEC0E3-48A3-4ECC-B913-F0DA248EEDBE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tipos de ambiente digite segun corresponda:
+-</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>laboratorio,salon,edificio,auditorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{C7FB44DC-8C15-4598-AD49-0BE5FC8BEA1A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Digite la facultad del ambiente: FIET,FIC</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G28" authorId="0" shapeId="0" xr:uid="{910AE657-1AFD-4A98-B5F2-14CC37FA7C1F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Recursos adicionales del ambiente:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+-Digite los recursos que tenga el ambiente separados por una coma.
+-Los recursos digitados deben estar previamente creados en la opcion agregar recursos de la aplicacion.
+-Si es un edificio se digita: 'no aplica'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H28" authorId="0" shapeId="0" xr:uid="{4B10E968-3778-4D2E-A0FC-B0CC0D7E99CE}">
       <text>
         <r>
           <rPr>
@@ -433,7 +610,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="48">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -504,14 +681,133 @@
     <t>Ejemplo</t>
   </si>
   <si>
-    <t>Se aceptan numeros de salones o nombres</t>
+    <t>Nombres de salones:</t>
+  </si>
+  <si>
+    <t>Nombres de laboratorios:</t>
+  </si>
+  <si>
+    <t>Mecanica</t>
+  </si>
+  <si>
+    <t>Primero se ingresa el nombre del edificio, luego se ingresa los salones y demas que lo compongan.</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>IPET</t>
+  </si>
+  <si>
+    <t>no aplica</t>
+  </si>
+  <si>
+    <t>Se aceptan numeros de salones o nombres.</t>
+  </si>
+  <si>
+    <t>Si el ambiente es de Tipo 'Edificio' en ubicacion es: no aplica</t>
+  </si>
+  <si>
+    <t>Si el ambiente es de Tipo 'Salon', 'Auditorio', 'Laboratorio' en ubicacion digite el edificio donde se encuentra.</t>
+  </si>
+  <si>
+    <t>Geotecnia</t>
+  </si>
+  <si>
+    <t>Si es Edificio: no aplica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digite la capacidad en numeros </t>
+  </si>
+  <si>
+    <t>Primero se ingresa el TIPO edificio Y luego se ingresa los salones,laboratorios o demas que lo compongan.</t>
+  </si>
+  <si>
+    <t>Suelos</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se selecciona las facultades disponibles descargadas desde la aplicacion web en la ventana </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CONSULTAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> puede ver el codigo correspondiente a la facultad.</t>
+    </r>
+  </si>
+  <si>
+    <t>Televisor, Video Beam</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Si es un solo recurso adicional se escribe como este en la tabla de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RECURSOS ADICIONALES DISPONIBLES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, si son varios se separan por coma.</t>
+    </r>
+  </si>
+  <si>
+    <t>Si es un solo recurso se coloca su cantidad, si son varios se separan por coma, si es edificio no aplica.</t>
+  </si>
+  <si>
+    <t>Computador</t>
+  </si>
+  <si>
+    <t>Caso de Ejecucion:</t>
+  </si>
+  <si>
+    <t>televisor, portatil</t>
+  </si>
+  <si>
+    <t>televisor, video beam</t>
+  </si>
+  <si>
+    <t>computador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,8 +857,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,6 +882,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,7 +919,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -635,26 +945,48 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -973,19 +1305,19 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.140625"/>
+    <col min="2" max="2" customWidth="true" width="15.0"/>
+    <col min="3" max="3" customWidth="true" style="4" width="15.5703125"/>
+    <col min="4" max="4" customWidth="true" width="13.28515625"/>
+    <col min="5" max="5" customWidth="true" width="10.0"/>
+    <col min="6" max="6" customWidth="true" width="26.85546875"/>
+    <col min="7" max="7" customWidth="true" style="5" width="16.7109375"/>
+    <col min="10" max="10" customWidth="true" width="31.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1046,7 +1378,9 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="9"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -1524,7 +1858,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6AF341C7-0E8B-4088-BCA7-B71A4E918A36}">
           <x14:formula1>
@@ -1532,7 +1866,7 @@
           </x14:formula1>
           <xm:sqref>E2:E51</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3AD9774D-9FF1-4400-B2B8-3828324770F9}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{683CE49D-FFD0-4AE2-82E2-8749F34F955F}">
           <x14:formula1>
             <xm:f>CONSULTAS!$E$2:$E$5</xm:f>
           </x14:formula1>
@@ -1546,95 +1880,687 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51C9D736-7310-4A2E-A36F-E6626D36506D}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C1" sqref="C1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.140625"/>
+    <col min="2" max="2" customWidth="true" width="23.5703125"/>
+    <col min="3" max="3" customWidth="true" width="14.140625"/>
+    <col min="5" max="5" customWidth="true" width="23.7109375"/>
+    <col min="6" max="6" customWidth="true" width="13.42578125"/>
+    <col min="7" max="7" customWidth="true" width="22.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="17">
+        <v>220</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="13">
+        <v>20</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+      <c r="B5" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="D5" s="17">
+        <v>220</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="4"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="B6" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="F6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="13">
+        <v>253</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="13">
+        <v>30</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="13">
+        <v>253</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="17">
+        <v>30</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="13">
+        <v>30</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="B15" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="B17" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
+    </row>
+    <row r="18" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="13">
+        <v>220</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="13">
+        <v>220</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="20"/>
+    </row>
+    <row r="28" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="19">
+        <v>4</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="8">
+        <v>30</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="19">
+        <v>322</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="8">
+        <v>30</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="19">
+        <v>210</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="8">
+        <v>25</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="19">
+        <v>4</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="8">
+        <v>30</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="19">
+        <v>322</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="8">
+        <v>30</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="19">
+        <v>210</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="8">
+        <v>25</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A010E52C-A240-4890-9DB7-404AE0E875E9}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50A2B91C-0D90-48F2-99CD-D22755E280B3}">
           <x14:formula1>
-            <xm:f>CONSULTAS!$E$2:$E$5</xm:f>
+            <xm:f>CONSULTAS!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>D3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9FA72875-C813-4610-8532-95DCADBDA22F}">
-          <x14:formula1>
-            <xm:f>CONSULTAS!$A$2:$A$20</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3</xm:sqref>
+          <xm:sqref>F16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1644,30 +2570,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B871DA-02F7-4B0C-AA3F-5422D277DFCC}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="59.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="59.5703125"/>
+    <col min="5" max="5" customWidth="true" width="14.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
@@ -1678,7 +2604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -1686,64 +2612,65 @@
         <v>14</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="E5" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
     </row>
@@ -1925,5 +2852,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>